<commit_message>
finished the excel functions
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chotd\Documents\Coding\Python\workLogger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6968828C-66FF-4F94-9B59-A8472225ED1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E08D1-74B1-489B-B990-F7432A84CE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Focus session</t>
+  </si>
+  <si>
+    <t>28/01/2025</t>
   </si>
 </sst>
 </file>
@@ -349,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,22 +374,55 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2">
+        <v>45686</v>
+      </c>
+      <c r="B4" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B6" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
integrated excel function into main file
finished excel functions, integrated into main file, improved the UI
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chotd\Documents\Coding\Python\workLogger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E08D1-74B1-489B-B990-F7432A84CE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0289C7-2E0D-4049-AAFD-975DE70CDC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
@@ -355,7 +355,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,12 +414,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>135</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>

</xml_diff>